<commit_message>
fully function uploading questions
</commit_message>
<xml_diff>
--- a/excel/question.xlsx
+++ b/excel/question.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="32">
   <si>
     <t>Whats your (full) name?</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>choice 8</t>
-  </si>
-  <si>
-    <t>2this is the answer</t>
   </si>
 </sst>
 </file>
@@ -442,60 +439,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -503,65 +498,59 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
       </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -569,88 +558,85 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
       <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -658,209 +644,203 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>23</v>
       </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
       <c r="D18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
       </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
       <c r="E19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
       <c r="E21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>